<commit_message>
Quick fix for return /r being added to last item
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lonjh73/projetcs/moltin-tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DB1B037-D828-DA41-ABF2-A9A2DE627D0D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E9F0AB4-7173-C348-BA14-6224AF9F5658}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2300" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{9C1E51AD-C946-5248-A5DD-253FC6FABADF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="products" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>name</t>
   </si>
@@ -55,6 +55,24 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>formatFix</t>
+  </si>
+  <si>
+    <t>manage_stock</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>test-product</t>
+  </si>
+  <si>
+    <t>sku</t>
+  </si>
+  <si>
+    <t>clitestproduct</t>
   </si>
 </sst>
 </file>
@@ -406,15 +424,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B1FF17-2D02-694F-90A7-9FBF3C9E06F0}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="7" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,10 +449,22 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -442,7 +475,16 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>1.99</v>
+        <v>199</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>